<commit_message>
End of Session: H-044 Context Helper System & Maintenance Expansion
</commit_message>
<xml_diff>
--- a/configs/table-configs/buildings-complete.xlsx
+++ b/configs/table-configs/buildings-complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edward/Dev/Nuxt/EE_manager/configs/table-configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52199F6C-491B-F648-9498-48B8DDEAD4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A0588D-A269-CC40-AD30-65AFBDA2A692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="162520" yWindow="14080" windowWidth="33560" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,7 +695,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,7 +875,7 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -903,7 +903,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 A6:E6 A2:B2 D2:J2 A3 D3:E3 A4:B4 D4:E4 G6:J6 G3:J3 G4:J4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 A6:B6 A2:B2 D2:J2 A3 D3:E3 A4:B4 D4:E4 G6:J6 G3:J3 G4:J4 D6:E6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>